<commit_message>
added chart 1,2 & table 1
</commit_message>
<xml_diff>
--- a/UK/1. Monthly-cape-ratios_UK.xlsx
+++ b/UK/1. Monthly-cape-ratios_UK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UW\2. Summer 22-23\3. Equity and Fixed Income\EFI_Homework\UK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A58FCEC-ED8E-46EE-AF74-D71780E46FCD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47E85CC-2918-4D09-88CB-0BCB2470C881}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6909,8 +6909,8 @@
   <dimension ref="A2:K498"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <pane ySplit="2" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J103" sqref="J103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>